<commit_message>
added plots function and code to get clean data
</commit_message>
<xml_diff>
--- a/hw2/sifma/US-Agency-Debt-Statistics-SIFMA.xlsx
+++ b/hw2/sifma/US-Agency-Debt-Statistics-SIFMA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Shared With Me\Research\Data\Data - Website\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guill\Desktop\financial_institutions\hw2\sifma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{253CDCB5-AC6E-4ED4-8946-EC93DA565F09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DB12742-6272-430B-93C5-CCA5F73AB7AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5295" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table of Contents" sheetId="7" r:id="rId1"/>
@@ -797,15 +797,15 @@
     <xf numFmtId="166" fontId="11" fillId="2" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="8" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="13" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="8" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="13" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="8" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="8" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="8" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="29" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1194,7 +1194,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:IU23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="12.75"/>
   <cols>
@@ -1416,220 +1418,220 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:255">
-      <c r="B1" s="96" t="s">
+      <c r="B1" s="99" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
-      <c r="K1" s="96"/>
-      <c r="M1" s="96"/>
-      <c r="N1" s="96"/>
-      <c r="O1" s="96"/>
-      <c r="P1" s="96"/>
-      <c r="Q1" s="96"/>
-      <c r="S1" s="96"/>
-      <c r="T1" s="96"/>
-      <c r="U1" s="96"/>
-      <c r="V1" s="96"/>
-      <c r="W1" s="96"/>
-      <c r="Y1" s="96"/>
-      <c r="Z1" s="96"/>
-      <c r="AA1" s="96"/>
-      <c r="AB1" s="96"/>
-      <c r="AC1" s="96"/>
-      <c r="AE1" s="96"/>
-      <c r="AF1" s="96"/>
-      <c r="AG1" s="96"/>
-      <c r="AH1" s="96"/>
-      <c r="AI1" s="96"/>
-      <c r="AK1" s="96"/>
-      <c r="AL1" s="96"/>
-      <c r="AM1" s="96"/>
-      <c r="AN1" s="96"/>
-      <c r="AO1" s="96"/>
-      <c r="AQ1" s="96"/>
-      <c r="AR1" s="96"/>
-      <c r="AS1" s="96"/>
-      <c r="AT1" s="96"/>
-      <c r="AU1" s="96"/>
-      <c r="AW1" s="96"/>
-      <c r="AX1" s="96"/>
-      <c r="AY1" s="96"/>
-      <c r="AZ1" s="96"/>
-      <c r="BA1" s="96"/>
-      <c r="BC1" s="96"/>
-      <c r="BD1" s="96"/>
-      <c r="BE1" s="96"/>
-      <c r="BF1" s="96"/>
-      <c r="BG1" s="96"/>
-      <c r="BI1" s="96"/>
-      <c r="BJ1" s="96"/>
-      <c r="BK1" s="96"/>
-      <c r="BL1" s="96"/>
-      <c r="BM1" s="96"/>
-      <c r="BO1" s="96"/>
-      <c r="BP1" s="96"/>
-      <c r="BQ1" s="96"/>
-      <c r="BR1" s="96"/>
-      <c r="BS1" s="96"/>
-      <c r="BU1" s="96"/>
-      <c r="BV1" s="96"/>
-      <c r="BW1" s="96"/>
-      <c r="BX1" s="96"/>
-      <c r="BY1" s="96"/>
-      <c r="CA1" s="96"/>
-      <c r="CB1" s="96"/>
-      <c r="CC1" s="96"/>
-      <c r="CD1" s="96"/>
-      <c r="CE1" s="96"/>
-      <c r="CG1" s="96"/>
-      <c r="CH1" s="96"/>
-      <c r="CI1" s="96"/>
-      <c r="CJ1" s="96"/>
-      <c r="CK1" s="96"/>
-      <c r="CM1" s="96"/>
-      <c r="CN1" s="96"/>
-      <c r="CO1" s="96"/>
-      <c r="CP1" s="96"/>
-      <c r="CQ1" s="96"/>
-      <c r="CS1" s="96"/>
-      <c r="CT1" s="96"/>
-      <c r="CU1" s="96"/>
-      <c r="CV1" s="96"/>
-      <c r="CW1" s="96"/>
-      <c r="CY1" s="96"/>
-      <c r="CZ1" s="96"/>
-      <c r="DA1" s="96"/>
-      <c r="DB1" s="96"/>
-      <c r="DC1" s="96"/>
-      <c r="DE1" s="96"/>
-      <c r="DF1" s="96"/>
-      <c r="DG1" s="96"/>
-      <c r="DH1" s="96"/>
-      <c r="DI1" s="96"/>
-      <c r="DK1" s="96"/>
-      <c r="DL1" s="96"/>
-      <c r="DM1" s="96"/>
-      <c r="DN1" s="96"/>
-      <c r="DO1" s="96"/>
-      <c r="DQ1" s="96"/>
-      <c r="DR1" s="96"/>
-      <c r="DS1" s="96"/>
-      <c r="DT1" s="96"/>
-      <c r="DU1" s="96"/>
-      <c r="DW1" s="96"/>
-      <c r="DX1" s="96"/>
-      <c r="DY1" s="96"/>
-      <c r="DZ1" s="96"/>
-      <c r="EA1" s="96"/>
-      <c r="EC1" s="96"/>
-      <c r="ED1" s="96"/>
-      <c r="EE1" s="96"/>
-      <c r="EF1" s="96"/>
-      <c r="EG1" s="96"/>
-      <c r="EI1" s="96"/>
-      <c r="EJ1" s="96"/>
-      <c r="EK1" s="96"/>
-      <c r="EL1" s="96"/>
-      <c r="EM1" s="96"/>
-      <c r="EO1" s="96"/>
-      <c r="EP1" s="96"/>
-      <c r="EQ1" s="96"/>
-      <c r="ER1" s="96"/>
-      <c r="ES1" s="96"/>
-      <c r="EU1" s="96"/>
-      <c r="EV1" s="96"/>
-      <c r="EW1" s="96"/>
-      <c r="EX1" s="96"/>
-      <c r="EY1" s="96"/>
-      <c r="FA1" s="96"/>
-      <c r="FB1" s="96"/>
-      <c r="FC1" s="96"/>
-      <c r="FD1" s="96"/>
-      <c r="FE1" s="96"/>
-      <c r="FG1" s="96"/>
-      <c r="FH1" s="96"/>
-      <c r="FI1" s="96"/>
-      <c r="FJ1" s="96"/>
-      <c r="FK1" s="96"/>
-      <c r="FM1" s="96"/>
-      <c r="FN1" s="96"/>
-      <c r="FO1" s="96"/>
-      <c r="FP1" s="96"/>
-      <c r="FQ1" s="96"/>
-      <c r="FS1" s="96"/>
-      <c r="FT1" s="96"/>
-      <c r="FU1" s="96"/>
-      <c r="FV1" s="96"/>
-      <c r="FW1" s="96"/>
-      <c r="FY1" s="96"/>
-      <c r="FZ1" s="96"/>
-      <c r="GA1" s="96"/>
-      <c r="GB1" s="96"/>
-      <c r="GC1" s="96"/>
-      <c r="GE1" s="96"/>
-      <c r="GF1" s="96"/>
-      <c r="GG1" s="96"/>
-      <c r="GH1" s="96"/>
-      <c r="GI1" s="96"/>
-      <c r="GK1" s="96"/>
-      <c r="GL1" s="96"/>
-      <c r="GM1" s="96"/>
-      <c r="GN1" s="96"/>
-      <c r="GO1" s="96"/>
-      <c r="GQ1" s="96"/>
-      <c r="GR1" s="96"/>
-      <c r="GS1" s="96"/>
-      <c r="GT1" s="96"/>
-      <c r="GU1" s="96"/>
-      <c r="GW1" s="96"/>
-      <c r="GX1" s="96"/>
-      <c r="GY1" s="96"/>
-      <c r="GZ1" s="96"/>
-      <c r="HA1" s="96"/>
-      <c r="HC1" s="96"/>
-      <c r="HD1" s="96"/>
-      <c r="HE1" s="96"/>
-      <c r="HF1" s="96"/>
-      <c r="HG1" s="96"/>
-      <c r="HI1" s="96"/>
-      <c r="HJ1" s="96"/>
-      <c r="HK1" s="96"/>
-      <c r="HL1" s="96"/>
-      <c r="HM1" s="96"/>
-      <c r="HO1" s="96"/>
-      <c r="HP1" s="96"/>
-      <c r="HQ1" s="96"/>
-      <c r="HR1" s="96"/>
-      <c r="HS1" s="96"/>
-      <c r="HU1" s="96"/>
-      <c r="HV1" s="96"/>
-      <c r="HW1" s="96"/>
-      <c r="HX1" s="96"/>
-      <c r="HY1" s="96"/>
-      <c r="IA1" s="96"/>
-      <c r="IB1" s="96"/>
-      <c r="IC1" s="96"/>
-      <c r="ID1" s="96"/>
-      <c r="IE1" s="96"/>
-      <c r="IG1" s="96"/>
-      <c r="IH1" s="96"/>
-      <c r="II1" s="96"/>
-      <c r="IJ1" s="96"/>
-      <c r="IK1" s="96"/>
-      <c r="IM1" s="96"/>
-      <c r="IN1" s="96"/>
-      <c r="IO1" s="96"/>
-      <c r="IP1" s="96"/>
-      <c r="IQ1" s="96"/>
-      <c r="IS1" s="96"/>
-      <c r="IT1" s="99"/>
-      <c r="IU1" s="99"/>
+      <c r="C1" s="99"/>
+      <c r="D1" s="99"/>
+      <c r="E1" s="99"/>
+      <c r="G1" s="99"/>
+      <c r="H1" s="99"/>
+      <c r="I1" s="99"/>
+      <c r="J1" s="99"/>
+      <c r="K1" s="99"/>
+      <c r="M1" s="99"/>
+      <c r="N1" s="99"/>
+      <c r="O1" s="99"/>
+      <c r="P1" s="99"/>
+      <c r="Q1" s="99"/>
+      <c r="S1" s="99"/>
+      <c r="T1" s="99"/>
+      <c r="U1" s="99"/>
+      <c r="V1" s="99"/>
+      <c r="W1" s="99"/>
+      <c r="Y1" s="99"/>
+      <c r="Z1" s="99"/>
+      <c r="AA1" s="99"/>
+      <c r="AB1" s="99"/>
+      <c r="AC1" s="99"/>
+      <c r="AE1" s="99"/>
+      <c r="AF1" s="99"/>
+      <c r="AG1" s="99"/>
+      <c r="AH1" s="99"/>
+      <c r="AI1" s="99"/>
+      <c r="AK1" s="99"/>
+      <c r="AL1" s="99"/>
+      <c r="AM1" s="99"/>
+      <c r="AN1" s="99"/>
+      <c r="AO1" s="99"/>
+      <c r="AQ1" s="99"/>
+      <c r="AR1" s="99"/>
+      <c r="AS1" s="99"/>
+      <c r="AT1" s="99"/>
+      <c r="AU1" s="99"/>
+      <c r="AW1" s="99"/>
+      <c r="AX1" s="99"/>
+      <c r="AY1" s="99"/>
+      <c r="AZ1" s="99"/>
+      <c r="BA1" s="99"/>
+      <c r="BC1" s="99"/>
+      <c r="BD1" s="99"/>
+      <c r="BE1" s="99"/>
+      <c r="BF1" s="99"/>
+      <c r="BG1" s="99"/>
+      <c r="BI1" s="99"/>
+      <c r="BJ1" s="99"/>
+      <c r="BK1" s="99"/>
+      <c r="BL1" s="99"/>
+      <c r="BM1" s="99"/>
+      <c r="BO1" s="99"/>
+      <c r="BP1" s="99"/>
+      <c r="BQ1" s="99"/>
+      <c r="BR1" s="99"/>
+      <c r="BS1" s="99"/>
+      <c r="BU1" s="99"/>
+      <c r="BV1" s="99"/>
+      <c r="BW1" s="99"/>
+      <c r="BX1" s="99"/>
+      <c r="BY1" s="99"/>
+      <c r="CA1" s="99"/>
+      <c r="CB1" s="99"/>
+      <c r="CC1" s="99"/>
+      <c r="CD1" s="99"/>
+      <c r="CE1" s="99"/>
+      <c r="CG1" s="99"/>
+      <c r="CH1" s="99"/>
+      <c r="CI1" s="99"/>
+      <c r="CJ1" s="99"/>
+      <c r="CK1" s="99"/>
+      <c r="CM1" s="99"/>
+      <c r="CN1" s="99"/>
+      <c r="CO1" s="99"/>
+      <c r="CP1" s="99"/>
+      <c r="CQ1" s="99"/>
+      <c r="CS1" s="99"/>
+      <c r="CT1" s="99"/>
+      <c r="CU1" s="99"/>
+      <c r="CV1" s="99"/>
+      <c r="CW1" s="99"/>
+      <c r="CY1" s="99"/>
+      <c r="CZ1" s="99"/>
+      <c r="DA1" s="99"/>
+      <c r="DB1" s="99"/>
+      <c r="DC1" s="99"/>
+      <c r="DE1" s="99"/>
+      <c r="DF1" s="99"/>
+      <c r="DG1" s="99"/>
+      <c r="DH1" s="99"/>
+      <c r="DI1" s="99"/>
+      <c r="DK1" s="99"/>
+      <c r="DL1" s="99"/>
+      <c r="DM1" s="99"/>
+      <c r="DN1" s="99"/>
+      <c r="DO1" s="99"/>
+      <c r="DQ1" s="99"/>
+      <c r="DR1" s="99"/>
+      <c r="DS1" s="99"/>
+      <c r="DT1" s="99"/>
+      <c r="DU1" s="99"/>
+      <c r="DW1" s="99"/>
+      <c r="DX1" s="99"/>
+      <c r="DY1" s="99"/>
+      <c r="DZ1" s="99"/>
+      <c r="EA1" s="99"/>
+      <c r="EC1" s="99"/>
+      <c r="ED1" s="99"/>
+      <c r="EE1" s="99"/>
+      <c r="EF1" s="99"/>
+      <c r="EG1" s="99"/>
+      <c r="EI1" s="99"/>
+      <c r="EJ1" s="99"/>
+      <c r="EK1" s="99"/>
+      <c r="EL1" s="99"/>
+      <c r="EM1" s="99"/>
+      <c r="EO1" s="99"/>
+      <c r="EP1" s="99"/>
+      <c r="EQ1" s="99"/>
+      <c r="ER1" s="99"/>
+      <c r="ES1" s="99"/>
+      <c r="EU1" s="99"/>
+      <c r="EV1" s="99"/>
+      <c r="EW1" s="99"/>
+      <c r="EX1" s="99"/>
+      <c r="EY1" s="99"/>
+      <c r="FA1" s="99"/>
+      <c r="FB1" s="99"/>
+      <c r="FC1" s="99"/>
+      <c r="FD1" s="99"/>
+      <c r="FE1" s="99"/>
+      <c r="FG1" s="99"/>
+      <c r="FH1" s="99"/>
+      <c r="FI1" s="99"/>
+      <c r="FJ1" s="99"/>
+      <c r="FK1" s="99"/>
+      <c r="FM1" s="99"/>
+      <c r="FN1" s="99"/>
+      <c r="FO1" s="99"/>
+      <c r="FP1" s="99"/>
+      <c r="FQ1" s="99"/>
+      <c r="FS1" s="99"/>
+      <c r="FT1" s="99"/>
+      <c r="FU1" s="99"/>
+      <c r="FV1" s="99"/>
+      <c r="FW1" s="99"/>
+      <c r="FY1" s="99"/>
+      <c r="FZ1" s="99"/>
+      <c r="GA1" s="99"/>
+      <c r="GB1" s="99"/>
+      <c r="GC1" s="99"/>
+      <c r="GE1" s="99"/>
+      <c r="GF1" s="99"/>
+      <c r="GG1" s="99"/>
+      <c r="GH1" s="99"/>
+      <c r="GI1" s="99"/>
+      <c r="GK1" s="99"/>
+      <c r="GL1" s="99"/>
+      <c r="GM1" s="99"/>
+      <c r="GN1" s="99"/>
+      <c r="GO1" s="99"/>
+      <c r="GQ1" s="99"/>
+      <c r="GR1" s="99"/>
+      <c r="GS1" s="99"/>
+      <c r="GT1" s="99"/>
+      <c r="GU1" s="99"/>
+      <c r="GW1" s="99"/>
+      <c r="GX1" s="99"/>
+      <c r="GY1" s="99"/>
+      <c r="GZ1" s="99"/>
+      <c r="HA1" s="99"/>
+      <c r="HC1" s="99"/>
+      <c r="HD1" s="99"/>
+      <c r="HE1" s="99"/>
+      <c r="HF1" s="99"/>
+      <c r="HG1" s="99"/>
+      <c r="HI1" s="99"/>
+      <c r="HJ1" s="99"/>
+      <c r="HK1" s="99"/>
+      <c r="HL1" s="99"/>
+      <c r="HM1" s="99"/>
+      <c r="HO1" s="99"/>
+      <c r="HP1" s="99"/>
+      <c r="HQ1" s="99"/>
+      <c r="HR1" s="99"/>
+      <c r="HS1" s="99"/>
+      <c r="HU1" s="99"/>
+      <c r="HV1" s="99"/>
+      <c r="HW1" s="99"/>
+      <c r="HX1" s="99"/>
+      <c r="HY1" s="99"/>
+      <c r="IA1" s="99"/>
+      <c r="IB1" s="99"/>
+      <c r="IC1" s="99"/>
+      <c r="ID1" s="99"/>
+      <c r="IE1" s="99"/>
+      <c r="IG1" s="99"/>
+      <c r="IH1" s="99"/>
+      <c r="II1" s="99"/>
+      <c r="IJ1" s="99"/>
+      <c r="IK1" s="99"/>
+      <c r="IM1" s="99"/>
+      <c r="IN1" s="99"/>
+      <c r="IO1" s="99"/>
+      <c r="IP1" s="99"/>
+      <c r="IQ1" s="99"/>
+      <c r="IS1" s="99"/>
+      <c r="IT1" s="100"/>
+      <c r="IU1" s="100"/>
     </row>
     <row r="2" spans="2:255">
       <c r="B2" s="15" t="s">
@@ -3014,8 +3016,8 @@
       <c r="IP19" s="98"/>
       <c r="IQ19" s="98"/>
       <c r="IS19" s="98"/>
-      <c r="IT19" s="100"/>
-      <c r="IU19" s="100"/>
+      <c r="IT19" s="97"/>
+      <c r="IU19" s="97"/>
     </row>
     <row r="20" spans="2:255" s="25" customFormat="1" ht="11.25" customHeight="1">
       <c r="B20" s="26"/>
@@ -3232,220 +3234,220 @@
       <c r="IU20" s="26"/>
     </row>
     <row r="21" spans="2:255" s="25" customFormat="1" ht="67.5" customHeight="1">
-      <c r="B21" s="97" t="s">
+      <c r="B21" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="97"/>
-      <c r="D21" s="97"/>
-      <c r="E21" s="97"/>
-      <c r="G21" s="97"/>
-      <c r="H21" s="97"/>
-      <c r="I21" s="97"/>
-      <c r="J21" s="97"/>
-      <c r="K21" s="97"/>
-      <c r="M21" s="97"/>
-      <c r="N21" s="97"/>
-      <c r="O21" s="97"/>
-      <c r="P21" s="97"/>
-      <c r="Q21" s="97"/>
-      <c r="S21" s="97"/>
-      <c r="T21" s="97"/>
-      <c r="U21" s="97"/>
-      <c r="V21" s="97"/>
-      <c r="W21" s="97"/>
-      <c r="Y21" s="97"/>
-      <c r="Z21" s="97"/>
-      <c r="AA21" s="97"/>
-      <c r="AB21" s="97"/>
-      <c r="AC21" s="97"/>
-      <c r="AE21" s="97"/>
-      <c r="AF21" s="97"/>
-      <c r="AG21" s="97"/>
-      <c r="AH21" s="97"/>
-      <c r="AI21" s="97"/>
-      <c r="AK21" s="97"/>
-      <c r="AL21" s="97"/>
-      <c r="AM21" s="97"/>
-      <c r="AN21" s="97"/>
-      <c r="AO21" s="97"/>
-      <c r="AQ21" s="97"/>
-      <c r="AR21" s="97"/>
-      <c r="AS21" s="97"/>
-      <c r="AT21" s="97"/>
-      <c r="AU21" s="97"/>
-      <c r="AW21" s="97"/>
-      <c r="AX21" s="97"/>
-      <c r="AY21" s="97"/>
-      <c r="AZ21" s="97"/>
-      <c r="BA21" s="97"/>
-      <c r="BC21" s="97"/>
-      <c r="BD21" s="97"/>
-      <c r="BE21" s="97"/>
-      <c r="BF21" s="97"/>
-      <c r="BG21" s="97"/>
-      <c r="BI21" s="97"/>
-      <c r="BJ21" s="97"/>
-      <c r="BK21" s="97"/>
-      <c r="BL21" s="97"/>
-      <c r="BM21" s="97"/>
-      <c r="BO21" s="97"/>
-      <c r="BP21" s="97"/>
-      <c r="BQ21" s="97"/>
-      <c r="BR21" s="97"/>
-      <c r="BS21" s="97"/>
-      <c r="BU21" s="97"/>
-      <c r="BV21" s="97"/>
-      <c r="BW21" s="97"/>
-      <c r="BX21" s="97"/>
-      <c r="BY21" s="97"/>
-      <c r="CA21" s="97"/>
-      <c r="CB21" s="97"/>
-      <c r="CC21" s="97"/>
-      <c r="CD21" s="97"/>
-      <c r="CE21" s="97"/>
-      <c r="CG21" s="97"/>
-      <c r="CH21" s="97"/>
-      <c r="CI21" s="97"/>
-      <c r="CJ21" s="97"/>
-      <c r="CK21" s="97"/>
-      <c r="CM21" s="97"/>
-      <c r="CN21" s="97"/>
-      <c r="CO21" s="97"/>
-      <c r="CP21" s="97"/>
-      <c r="CQ21" s="97"/>
-      <c r="CS21" s="97"/>
-      <c r="CT21" s="97"/>
-      <c r="CU21" s="97"/>
-      <c r="CV21" s="97"/>
-      <c r="CW21" s="97"/>
-      <c r="CY21" s="97"/>
-      <c r="CZ21" s="97"/>
-      <c r="DA21" s="97"/>
-      <c r="DB21" s="97"/>
-      <c r="DC21" s="97"/>
-      <c r="DE21" s="97"/>
-      <c r="DF21" s="97"/>
-      <c r="DG21" s="97"/>
-      <c r="DH21" s="97"/>
-      <c r="DI21" s="97"/>
-      <c r="DK21" s="97"/>
-      <c r="DL21" s="97"/>
-      <c r="DM21" s="97"/>
-      <c r="DN21" s="97"/>
-      <c r="DO21" s="97"/>
-      <c r="DQ21" s="97"/>
-      <c r="DR21" s="97"/>
-      <c r="DS21" s="97"/>
-      <c r="DT21" s="97"/>
-      <c r="DU21" s="97"/>
-      <c r="DW21" s="97"/>
-      <c r="DX21" s="97"/>
-      <c r="DY21" s="97"/>
-      <c r="DZ21" s="97"/>
-      <c r="EA21" s="97"/>
-      <c r="EC21" s="97"/>
-      <c r="ED21" s="97"/>
-      <c r="EE21" s="97"/>
-      <c r="EF21" s="97"/>
-      <c r="EG21" s="97"/>
-      <c r="EI21" s="97"/>
-      <c r="EJ21" s="97"/>
-      <c r="EK21" s="97"/>
-      <c r="EL21" s="97"/>
-      <c r="EM21" s="97"/>
-      <c r="EO21" s="97"/>
-      <c r="EP21" s="97"/>
-      <c r="EQ21" s="97"/>
-      <c r="ER21" s="97"/>
-      <c r="ES21" s="97"/>
-      <c r="EU21" s="97"/>
-      <c r="EV21" s="97"/>
-      <c r="EW21" s="97"/>
-      <c r="EX21" s="97"/>
-      <c r="EY21" s="97"/>
-      <c r="FA21" s="97"/>
-      <c r="FB21" s="97"/>
-      <c r="FC21" s="97"/>
-      <c r="FD21" s="97"/>
-      <c r="FE21" s="97"/>
-      <c r="FG21" s="97"/>
-      <c r="FH21" s="97"/>
-      <c r="FI21" s="97"/>
-      <c r="FJ21" s="97"/>
-      <c r="FK21" s="97"/>
-      <c r="FM21" s="97"/>
-      <c r="FN21" s="97"/>
-      <c r="FO21" s="97"/>
-      <c r="FP21" s="97"/>
-      <c r="FQ21" s="97"/>
-      <c r="FS21" s="97"/>
-      <c r="FT21" s="97"/>
-      <c r="FU21" s="97"/>
-      <c r="FV21" s="97"/>
-      <c r="FW21" s="97"/>
-      <c r="FY21" s="97"/>
-      <c r="FZ21" s="97"/>
-      <c r="GA21" s="97"/>
-      <c r="GB21" s="97"/>
-      <c r="GC21" s="97"/>
-      <c r="GE21" s="97"/>
-      <c r="GF21" s="97"/>
-      <c r="GG21" s="97"/>
-      <c r="GH21" s="97"/>
-      <c r="GI21" s="97"/>
-      <c r="GK21" s="97"/>
-      <c r="GL21" s="97"/>
-      <c r="GM21" s="97"/>
-      <c r="GN21" s="97"/>
-      <c r="GO21" s="97"/>
-      <c r="GQ21" s="97"/>
-      <c r="GR21" s="97"/>
-      <c r="GS21" s="97"/>
-      <c r="GT21" s="97"/>
-      <c r="GU21" s="97"/>
-      <c r="GW21" s="97"/>
-      <c r="GX21" s="97"/>
-      <c r="GY21" s="97"/>
-      <c r="GZ21" s="97"/>
-      <c r="HA21" s="97"/>
-      <c r="HC21" s="97"/>
-      <c r="HD21" s="97"/>
-      <c r="HE21" s="97"/>
-      <c r="HF21" s="97"/>
-      <c r="HG21" s="97"/>
-      <c r="HI21" s="97"/>
-      <c r="HJ21" s="97"/>
-      <c r="HK21" s="97"/>
-      <c r="HL21" s="97"/>
-      <c r="HM21" s="97"/>
-      <c r="HO21" s="97"/>
-      <c r="HP21" s="97"/>
-      <c r="HQ21" s="97"/>
-      <c r="HR21" s="97"/>
-      <c r="HS21" s="97"/>
-      <c r="HU21" s="97"/>
-      <c r="HV21" s="97"/>
-      <c r="HW21" s="97"/>
-      <c r="HX21" s="97"/>
-      <c r="HY21" s="97"/>
-      <c r="IA21" s="97"/>
-      <c r="IB21" s="97"/>
-      <c r="IC21" s="97"/>
-      <c r="ID21" s="97"/>
-      <c r="IE21" s="97"/>
-      <c r="IG21" s="97"/>
-      <c r="IH21" s="97"/>
-      <c r="II21" s="97"/>
-      <c r="IJ21" s="97"/>
-      <c r="IK21" s="97"/>
-      <c r="IM21" s="97"/>
-      <c r="IN21" s="97"/>
-      <c r="IO21" s="97"/>
-      <c r="IP21" s="97"/>
-      <c r="IQ21" s="97"/>
-      <c r="IS21" s="97"/>
-      <c r="IT21" s="100"/>
-      <c r="IU21" s="100"/>
+      <c r="C21" s="96"/>
+      <c r="D21" s="96"/>
+      <c r="E21" s="96"/>
+      <c r="G21" s="96"/>
+      <c r="H21" s="96"/>
+      <c r="I21" s="96"/>
+      <c r="J21" s="96"/>
+      <c r="K21" s="96"/>
+      <c r="M21" s="96"/>
+      <c r="N21" s="96"/>
+      <c r="O21" s="96"/>
+      <c r="P21" s="96"/>
+      <c r="Q21" s="96"/>
+      <c r="S21" s="96"/>
+      <c r="T21" s="96"/>
+      <c r="U21" s="96"/>
+      <c r="V21" s="96"/>
+      <c r="W21" s="96"/>
+      <c r="Y21" s="96"/>
+      <c r="Z21" s="96"/>
+      <c r="AA21" s="96"/>
+      <c r="AB21" s="96"/>
+      <c r="AC21" s="96"/>
+      <c r="AE21" s="96"/>
+      <c r="AF21" s="96"/>
+      <c r="AG21" s="96"/>
+      <c r="AH21" s="96"/>
+      <c r="AI21" s="96"/>
+      <c r="AK21" s="96"/>
+      <c r="AL21" s="96"/>
+      <c r="AM21" s="96"/>
+      <c r="AN21" s="96"/>
+      <c r="AO21" s="96"/>
+      <c r="AQ21" s="96"/>
+      <c r="AR21" s="96"/>
+      <c r="AS21" s="96"/>
+      <c r="AT21" s="96"/>
+      <c r="AU21" s="96"/>
+      <c r="AW21" s="96"/>
+      <c r="AX21" s="96"/>
+      <c r="AY21" s="96"/>
+      <c r="AZ21" s="96"/>
+      <c r="BA21" s="96"/>
+      <c r="BC21" s="96"/>
+      <c r="BD21" s="96"/>
+      <c r="BE21" s="96"/>
+      <c r="BF21" s="96"/>
+      <c r="BG21" s="96"/>
+      <c r="BI21" s="96"/>
+      <c r="BJ21" s="96"/>
+      <c r="BK21" s="96"/>
+      <c r="BL21" s="96"/>
+      <c r="BM21" s="96"/>
+      <c r="BO21" s="96"/>
+      <c r="BP21" s="96"/>
+      <c r="BQ21" s="96"/>
+      <c r="BR21" s="96"/>
+      <c r="BS21" s="96"/>
+      <c r="BU21" s="96"/>
+      <c r="BV21" s="96"/>
+      <c r="BW21" s="96"/>
+      <c r="BX21" s="96"/>
+      <c r="BY21" s="96"/>
+      <c r="CA21" s="96"/>
+      <c r="CB21" s="96"/>
+      <c r="CC21" s="96"/>
+      <c r="CD21" s="96"/>
+      <c r="CE21" s="96"/>
+      <c r="CG21" s="96"/>
+      <c r="CH21" s="96"/>
+      <c r="CI21" s="96"/>
+      <c r="CJ21" s="96"/>
+      <c r="CK21" s="96"/>
+      <c r="CM21" s="96"/>
+      <c r="CN21" s="96"/>
+      <c r="CO21" s="96"/>
+      <c r="CP21" s="96"/>
+      <c r="CQ21" s="96"/>
+      <c r="CS21" s="96"/>
+      <c r="CT21" s="96"/>
+      <c r="CU21" s="96"/>
+      <c r="CV21" s="96"/>
+      <c r="CW21" s="96"/>
+      <c r="CY21" s="96"/>
+      <c r="CZ21" s="96"/>
+      <c r="DA21" s="96"/>
+      <c r="DB21" s="96"/>
+      <c r="DC21" s="96"/>
+      <c r="DE21" s="96"/>
+      <c r="DF21" s="96"/>
+      <c r="DG21" s="96"/>
+      <c r="DH21" s="96"/>
+      <c r="DI21" s="96"/>
+      <c r="DK21" s="96"/>
+      <c r="DL21" s="96"/>
+      <c r="DM21" s="96"/>
+      <c r="DN21" s="96"/>
+      <c r="DO21" s="96"/>
+      <c r="DQ21" s="96"/>
+      <c r="DR21" s="96"/>
+      <c r="DS21" s="96"/>
+      <c r="DT21" s="96"/>
+      <c r="DU21" s="96"/>
+      <c r="DW21" s="96"/>
+      <c r="DX21" s="96"/>
+      <c r="DY21" s="96"/>
+      <c r="DZ21" s="96"/>
+      <c r="EA21" s="96"/>
+      <c r="EC21" s="96"/>
+      <c r="ED21" s="96"/>
+      <c r="EE21" s="96"/>
+      <c r="EF21" s="96"/>
+      <c r="EG21" s="96"/>
+      <c r="EI21" s="96"/>
+      <c r="EJ21" s="96"/>
+      <c r="EK21" s="96"/>
+      <c r="EL21" s="96"/>
+      <c r="EM21" s="96"/>
+      <c r="EO21" s="96"/>
+      <c r="EP21" s="96"/>
+      <c r="EQ21" s="96"/>
+      <c r="ER21" s="96"/>
+      <c r="ES21" s="96"/>
+      <c r="EU21" s="96"/>
+      <c r="EV21" s="96"/>
+      <c r="EW21" s="96"/>
+      <c r="EX21" s="96"/>
+      <c r="EY21" s="96"/>
+      <c r="FA21" s="96"/>
+      <c r="FB21" s="96"/>
+      <c r="FC21" s="96"/>
+      <c r="FD21" s="96"/>
+      <c r="FE21" s="96"/>
+      <c r="FG21" s="96"/>
+      <c r="FH21" s="96"/>
+      <c r="FI21" s="96"/>
+      <c r="FJ21" s="96"/>
+      <c r="FK21" s="96"/>
+      <c r="FM21" s="96"/>
+      <c r="FN21" s="96"/>
+      <c r="FO21" s="96"/>
+      <c r="FP21" s="96"/>
+      <c r="FQ21" s="96"/>
+      <c r="FS21" s="96"/>
+      <c r="FT21" s="96"/>
+      <c r="FU21" s="96"/>
+      <c r="FV21" s="96"/>
+      <c r="FW21" s="96"/>
+      <c r="FY21" s="96"/>
+      <c r="FZ21" s="96"/>
+      <c r="GA21" s="96"/>
+      <c r="GB21" s="96"/>
+      <c r="GC21" s="96"/>
+      <c r="GE21" s="96"/>
+      <c r="GF21" s="96"/>
+      <c r="GG21" s="96"/>
+      <c r="GH21" s="96"/>
+      <c r="GI21" s="96"/>
+      <c r="GK21" s="96"/>
+      <c r="GL21" s="96"/>
+      <c r="GM21" s="96"/>
+      <c r="GN21" s="96"/>
+      <c r="GO21" s="96"/>
+      <c r="GQ21" s="96"/>
+      <c r="GR21" s="96"/>
+      <c r="GS21" s="96"/>
+      <c r="GT21" s="96"/>
+      <c r="GU21" s="96"/>
+      <c r="GW21" s="96"/>
+      <c r="GX21" s="96"/>
+      <c r="GY21" s="96"/>
+      <c r="GZ21" s="96"/>
+      <c r="HA21" s="96"/>
+      <c r="HC21" s="96"/>
+      <c r="HD21" s="96"/>
+      <c r="HE21" s="96"/>
+      <c r="HF21" s="96"/>
+      <c r="HG21" s="96"/>
+      <c r="HI21" s="96"/>
+      <c r="HJ21" s="96"/>
+      <c r="HK21" s="96"/>
+      <c r="HL21" s="96"/>
+      <c r="HM21" s="96"/>
+      <c r="HO21" s="96"/>
+      <c r="HP21" s="96"/>
+      <c r="HQ21" s="96"/>
+      <c r="HR21" s="96"/>
+      <c r="HS21" s="96"/>
+      <c r="HU21" s="96"/>
+      <c r="HV21" s="96"/>
+      <c r="HW21" s="96"/>
+      <c r="HX21" s="96"/>
+      <c r="HY21" s="96"/>
+      <c r="IA21" s="96"/>
+      <c r="IB21" s="96"/>
+      <c r="IC21" s="96"/>
+      <c r="ID21" s="96"/>
+      <c r="IE21" s="96"/>
+      <c r="IG21" s="96"/>
+      <c r="IH21" s="96"/>
+      <c r="II21" s="96"/>
+      <c r="IJ21" s="96"/>
+      <c r="IK21" s="96"/>
+      <c r="IM21" s="96"/>
+      <c r="IN21" s="96"/>
+      <c r="IO21" s="96"/>
+      <c r="IP21" s="96"/>
+      <c r="IQ21" s="96"/>
+      <c r="IS21" s="96"/>
+      <c r="IT21" s="97"/>
+      <c r="IU21" s="97"/>
     </row>
     <row r="22" spans="2:255" s="25" customFormat="1" ht="11.25" customHeight="1">
       <c r="B22" s="26"/>
@@ -3662,296 +3664,298 @@
       <c r="IU22" s="26"/>
     </row>
     <row r="23" spans="2:255" s="25" customFormat="1" ht="11.25" customHeight="1">
-      <c r="B23" s="97" t="s">
+      <c r="B23" s="96" t="s">
         <v>33</v>
       </c>
-      <c r="C23" s="97"/>
-      <c r="D23" s="97"/>
-      <c r="E23" s="97"/>
-      <c r="G23" s="97"/>
-      <c r="H23" s="97"/>
-      <c r="I23" s="97"/>
-      <c r="J23" s="97"/>
-      <c r="K23" s="97"/>
-      <c r="M23" s="97"/>
-      <c r="N23" s="97"/>
-      <c r="O23" s="97"/>
-      <c r="P23" s="97"/>
-      <c r="Q23" s="97"/>
-      <c r="S23" s="97"/>
-      <c r="T23" s="97"/>
-      <c r="U23" s="97"/>
-      <c r="V23" s="97"/>
-      <c r="W23" s="97"/>
-      <c r="Y23" s="97"/>
-      <c r="Z23" s="97"/>
-      <c r="AA23" s="97"/>
-      <c r="AB23" s="97"/>
-      <c r="AC23" s="97"/>
-      <c r="AE23" s="97"/>
-      <c r="AF23" s="97"/>
-      <c r="AG23" s="97"/>
-      <c r="AH23" s="97"/>
-      <c r="AI23" s="97"/>
-      <c r="AK23" s="97"/>
-      <c r="AL23" s="97"/>
-      <c r="AM23" s="97"/>
-      <c r="AN23" s="97"/>
-      <c r="AO23" s="97"/>
-      <c r="AQ23" s="97"/>
-      <c r="AR23" s="97"/>
-      <c r="AS23" s="97"/>
-      <c r="AT23" s="97"/>
-      <c r="AU23" s="97"/>
-      <c r="AW23" s="97"/>
-      <c r="AX23" s="97"/>
-      <c r="AY23" s="97"/>
-      <c r="AZ23" s="97"/>
-      <c r="BA23" s="97"/>
-      <c r="BC23" s="97"/>
-      <c r="BD23" s="97"/>
-      <c r="BE23" s="97"/>
-      <c r="BF23" s="97"/>
-      <c r="BG23" s="97"/>
-      <c r="BI23" s="97"/>
-      <c r="BJ23" s="97"/>
-      <c r="BK23" s="97"/>
-      <c r="BL23" s="97"/>
-      <c r="BM23" s="97"/>
-      <c r="BO23" s="97"/>
-      <c r="BP23" s="97"/>
-      <c r="BQ23" s="97"/>
-      <c r="BR23" s="97"/>
-      <c r="BS23" s="97"/>
-      <c r="BU23" s="97"/>
-      <c r="BV23" s="97"/>
-      <c r="BW23" s="97"/>
-      <c r="BX23" s="97"/>
-      <c r="BY23" s="97"/>
-      <c r="CA23" s="97"/>
-      <c r="CB23" s="97"/>
-      <c r="CC23" s="97"/>
-      <c r="CD23" s="97"/>
-      <c r="CE23" s="97"/>
-      <c r="CG23" s="97"/>
-      <c r="CH23" s="97"/>
-      <c r="CI23" s="97"/>
-      <c r="CJ23" s="97"/>
-      <c r="CK23" s="97"/>
-      <c r="CM23" s="97"/>
-      <c r="CN23" s="97"/>
-      <c r="CO23" s="97"/>
-      <c r="CP23" s="97"/>
-      <c r="CQ23" s="97"/>
-      <c r="CS23" s="97"/>
-      <c r="CT23" s="97"/>
-      <c r="CU23" s="97"/>
-      <c r="CV23" s="97"/>
-      <c r="CW23" s="97"/>
-      <c r="CY23" s="97"/>
-      <c r="CZ23" s="97"/>
-      <c r="DA23" s="97"/>
-      <c r="DB23" s="97"/>
-      <c r="DC23" s="97"/>
-      <c r="DE23" s="97"/>
-      <c r="DF23" s="97"/>
-      <c r="DG23" s="97"/>
-      <c r="DH23" s="97"/>
-      <c r="DI23" s="97"/>
-      <c r="DK23" s="97"/>
-      <c r="DL23" s="97"/>
-      <c r="DM23" s="97"/>
-      <c r="DN23" s="97"/>
-      <c r="DO23" s="97"/>
-      <c r="DQ23" s="97"/>
-      <c r="DR23" s="97"/>
-      <c r="DS23" s="97"/>
-      <c r="DT23" s="97"/>
-      <c r="DU23" s="97"/>
-      <c r="DW23" s="97"/>
-      <c r="DX23" s="97"/>
-      <c r="DY23" s="97"/>
-      <c r="DZ23" s="97"/>
-      <c r="EA23" s="97"/>
-      <c r="EC23" s="97"/>
-      <c r="ED23" s="97"/>
-      <c r="EE23" s="97"/>
-      <c r="EF23" s="97"/>
-      <c r="EG23" s="97"/>
-      <c r="EI23" s="97"/>
-      <c r="EJ23" s="97"/>
-      <c r="EK23" s="97"/>
-      <c r="EL23" s="97"/>
-      <c r="EM23" s="97"/>
-      <c r="EO23" s="97"/>
-      <c r="EP23" s="97"/>
-      <c r="EQ23" s="97"/>
-      <c r="ER23" s="97"/>
-      <c r="ES23" s="97"/>
-      <c r="EU23" s="97"/>
-      <c r="EV23" s="97"/>
-      <c r="EW23" s="97"/>
-      <c r="EX23" s="97"/>
-      <c r="EY23" s="97"/>
-      <c r="FA23" s="97"/>
-      <c r="FB23" s="97"/>
-      <c r="FC23" s="97"/>
-      <c r="FD23" s="97"/>
-      <c r="FE23" s="97"/>
-      <c r="FG23" s="97"/>
-      <c r="FH23" s="97"/>
-      <c r="FI23" s="97"/>
-      <c r="FJ23" s="97"/>
-      <c r="FK23" s="97"/>
-      <c r="FM23" s="97"/>
-      <c r="FN23" s="97"/>
-      <c r="FO23" s="97"/>
-      <c r="FP23" s="97"/>
-      <c r="FQ23" s="97"/>
-      <c r="FS23" s="97"/>
-      <c r="FT23" s="97"/>
-      <c r="FU23" s="97"/>
-      <c r="FV23" s="97"/>
-      <c r="FW23" s="97"/>
-      <c r="FY23" s="97"/>
-      <c r="FZ23" s="97"/>
-      <c r="GA23" s="97"/>
-      <c r="GB23" s="97"/>
-      <c r="GC23" s="97"/>
-      <c r="GE23" s="97"/>
-      <c r="GF23" s="97"/>
-      <c r="GG23" s="97"/>
-      <c r="GH23" s="97"/>
-      <c r="GI23" s="97"/>
-      <c r="GK23" s="97"/>
-      <c r="GL23" s="97"/>
-      <c r="GM23" s="97"/>
-      <c r="GN23" s="97"/>
-      <c r="GO23" s="97"/>
-      <c r="GQ23" s="97"/>
-      <c r="GR23" s="97"/>
-      <c r="GS23" s="97"/>
-      <c r="GT23" s="97"/>
-      <c r="GU23" s="97"/>
-      <c r="GW23" s="97"/>
-      <c r="GX23" s="97"/>
-      <c r="GY23" s="97"/>
-      <c r="GZ23" s="97"/>
-      <c r="HA23" s="97"/>
-      <c r="HC23" s="97"/>
-      <c r="HD23" s="97"/>
-      <c r="HE23" s="97"/>
-      <c r="HF23" s="97"/>
-      <c r="HG23" s="97"/>
-      <c r="HI23" s="97"/>
-      <c r="HJ23" s="97"/>
-      <c r="HK23" s="97"/>
-      <c r="HL23" s="97"/>
-      <c r="HM23" s="97"/>
-      <c r="HO23" s="97"/>
-      <c r="HP23" s="97"/>
-      <c r="HQ23" s="97"/>
-      <c r="HR23" s="97"/>
-      <c r="HS23" s="97"/>
-      <c r="HU23" s="97"/>
-      <c r="HV23" s="97"/>
-      <c r="HW23" s="97"/>
-      <c r="HX23" s="97"/>
-      <c r="HY23" s="97"/>
-      <c r="IA23" s="97"/>
-      <c r="IB23" s="97"/>
-      <c r="IC23" s="97"/>
-      <c r="ID23" s="97"/>
-      <c r="IE23" s="97"/>
-      <c r="IG23" s="97"/>
-      <c r="IH23" s="97"/>
-      <c r="II23" s="97"/>
-      <c r="IJ23" s="97"/>
-      <c r="IK23" s="97"/>
-      <c r="IM23" s="97"/>
-      <c r="IN23" s="97"/>
-      <c r="IO23" s="97"/>
-      <c r="IP23" s="97"/>
-      <c r="IQ23" s="97"/>
-      <c r="IS23" s="97"/>
-      <c r="IT23" s="100"/>
-      <c r="IU23" s="100"/>
+      <c r="C23" s="96"/>
+      <c r="D23" s="96"/>
+      <c r="E23" s="96"/>
+      <c r="G23" s="96"/>
+      <c r="H23" s="96"/>
+      <c r="I23" s="96"/>
+      <c r="J23" s="96"/>
+      <c r="K23" s="96"/>
+      <c r="M23" s="96"/>
+      <c r="N23" s="96"/>
+      <c r="O23" s="96"/>
+      <c r="P23" s="96"/>
+      <c r="Q23" s="96"/>
+      <c r="S23" s="96"/>
+      <c r="T23" s="96"/>
+      <c r="U23" s="96"/>
+      <c r="V23" s="96"/>
+      <c r="W23" s="96"/>
+      <c r="Y23" s="96"/>
+      <c r="Z23" s="96"/>
+      <c r="AA23" s="96"/>
+      <c r="AB23" s="96"/>
+      <c r="AC23" s="96"/>
+      <c r="AE23" s="96"/>
+      <c r="AF23" s="96"/>
+      <c r="AG23" s="96"/>
+      <c r="AH23" s="96"/>
+      <c r="AI23" s="96"/>
+      <c r="AK23" s="96"/>
+      <c r="AL23" s="96"/>
+      <c r="AM23" s="96"/>
+      <c r="AN23" s="96"/>
+      <c r="AO23" s="96"/>
+      <c r="AQ23" s="96"/>
+      <c r="AR23" s="96"/>
+      <c r="AS23" s="96"/>
+      <c r="AT23" s="96"/>
+      <c r="AU23" s="96"/>
+      <c r="AW23" s="96"/>
+      <c r="AX23" s="96"/>
+      <c r="AY23" s="96"/>
+      <c r="AZ23" s="96"/>
+      <c r="BA23" s="96"/>
+      <c r="BC23" s="96"/>
+      <c r="BD23" s="96"/>
+      <c r="BE23" s="96"/>
+      <c r="BF23" s="96"/>
+      <c r="BG23" s="96"/>
+      <c r="BI23" s="96"/>
+      <c r="BJ23" s="96"/>
+      <c r="BK23" s="96"/>
+      <c r="BL23" s="96"/>
+      <c r="BM23" s="96"/>
+      <c r="BO23" s="96"/>
+      <c r="BP23" s="96"/>
+      <c r="BQ23" s="96"/>
+      <c r="BR23" s="96"/>
+      <c r="BS23" s="96"/>
+      <c r="BU23" s="96"/>
+      <c r="BV23" s="96"/>
+      <c r="BW23" s="96"/>
+      <c r="BX23" s="96"/>
+      <c r="BY23" s="96"/>
+      <c r="CA23" s="96"/>
+      <c r="CB23" s="96"/>
+      <c r="CC23" s="96"/>
+      <c r="CD23" s="96"/>
+      <c r="CE23" s="96"/>
+      <c r="CG23" s="96"/>
+      <c r="CH23" s="96"/>
+      <c r="CI23" s="96"/>
+      <c r="CJ23" s="96"/>
+      <c r="CK23" s="96"/>
+      <c r="CM23" s="96"/>
+      <c r="CN23" s="96"/>
+      <c r="CO23" s="96"/>
+      <c r="CP23" s="96"/>
+      <c r="CQ23" s="96"/>
+      <c r="CS23" s="96"/>
+      <c r="CT23" s="96"/>
+      <c r="CU23" s="96"/>
+      <c r="CV23" s="96"/>
+      <c r="CW23" s="96"/>
+      <c r="CY23" s="96"/>
+      <c r="CZ23" s="96"/>
+      <c r="DA23" s="96"/>
+      <c r="DB23" s="96"/>
+      <c r="DC23" s="96"/>
+      <c r="DE23" s="96"/>
+      <c r="DF23" s="96"/>
+      <c r="DG23" s="96"/>
+      <c r="DH23" s="96"/>
+      <c r="DI23" s="96"/>
+      <c r="DK23" s="96"/>
+      <c r="DL23" s="96"/>
+      <c r="DM23" s="96"/>
+      <c r="DN23" s="96"/>
+      <c r="DO23" s="96"/>
+      <c r="DQ23" s="96"/>
+      <c r="DR23" s="96"/>
+      <c r="DS23" s="96"/>
+      <c r="DT23" s="96"/>
+      <c r="DU23" s="96"/>
+      <c r="DW23" s="96"/>
+      <c r="DX23" s="96"/>
+      <c r="DY23" s="96"/>
+      <c r="DZ23" s="96"/>
+      <c r="EA23" s="96"/>
+      <c r="EC23" s="96"/>
+      <c r="ED23" s="96"/>
+      <c r="EE23" s="96"/>
+      <c r="EF23" s="96"/>
+      <c r="EG23" s="96"/>
+      <c r="EI23" s="96"/>
+      <c r="EJ23" s="96"/>
+      <c r="EK23" s="96"/>
+      <c r="EL23" s="96"/>
+      <c r="EM23" s="96"/>
+      <c r="EO23" s="96"/>
+      <c r="EP23" s="96"/>
+      <c r="EQ23" s="96"/>
+      <c r="ER23" s="96"/>
+      <c r="ES23" s="96"/>
+      <c r="EU23" s="96"/>
+      <c r="EV23" s="96"/>
+      <c r="EW23" s="96"/>
+      <c r="EX23" s="96"/>
+      <c r="EY23" s="96"/>
+      <c r="FA23" s="96"/>
+      <c r="FB23" s="96"/>
+      <c r="FC23" s="96"/>
+      <c r="FD23" s="96"/>
+      <c r="FE23" s="96"/>
+      <c r="FG23" s="96"/>
+      <c r="FH23" s="96"/>
+      <c r="FI23" s="96"/>
+      <c r="FJ23" s="96"/>
+      <c r="FK23" s="96"/>
+      <c r="FM23" s="96"/>
+      <c r="FN23" s="96"/>
+      <c r="FO23" s="96"/>
+      <c r="FP23" s="96"/>
+      <c r="FQ23" s="96"/>
+      <c r="FS23" s="96"/>
+      <c r="FT23" s="96"/>
+      <c r="FU23" s="96"/>
+      <c r="FV23" s="96"/>
+      <c r="FW23" s="96"/>
+      <c r="FY23" s="96"/>
+      <c r="FZ23" s="96"/>
+      <c r="GA23" s="96"/>
+      <c r="GB23" s="96"/>
+      <c r="GC23" s="96"/>
+      <c r="GE23" s="96"/>
+      <c r="GF23" s="96"/>
+      <c r="GG23" s="96"/>
+      <c r="GH23" s="96"/>
+      <c r="GI23" s="96"/>
+      <c r="GK23" s="96"/>
+      <c r="GL23" s="96"/>
+      <c r="GM23" s="96"/>
+      <c r="GN23" s="96"/>
+      <c r="GO23" s="96"/>
+      <c r="GQ23" s="96"/>
+      <c r="GR23" s="96"/>
+      <c r="GS23" s="96"/>
+      <c r="GT23" s="96"/>
+      <c r="GU23" s="96"/>
+      <c r="GW23" s="96"/>
+      <c r="GX23" s="96"/>
+      <c r="GY23" s="96"/>
+      <c r="GZ23" s="96"/>
+      <c r="HA23" s="96"/>
+      <c r="HC23" s="96"/>
+      <c r="HD23" s="96"/>
+      <c r="HE23" s="96"/>
+      <c r="HF23" s="96"/>
+      <c r="HG23" s="96"/>
+      <c r="HI23" s="96"/>
+      <c r="HJ23" s="96"/>
+      <c r="HK23" s="96"/>
+      <c r="HL23" s="96"/>
+      <c r="HM23" s="96"/>
+      <c r="HO23" s="96"/>
+      <c r="HP23" s="96"/>
+      <c r="HQ23" s="96"/>
+      <c r="HR23" s="96"/>
+      <c r="HS23" s="96"/>
+      <c r="HU23" s="96"/>
+      <c r="HV23" s="96"/>
+      <c r="HW23" s="96"/>
+      <c r="HX23" s="96"/>
+      <c r="HY23" s="96"/>
+      <c r="IA23" s="96"/>
+      <c r="IB23" s="96"/>
+      <c r="IC23" s="96"/>
+      <c r="ID23" s="96"/>
+      <c r="IE23" s="96"/>
+      <c r="IG23" s="96"/>
+      <c r="IH23" s="96"/>
+      <c r="II23" s="96"/>
+      <c r="IJ23" s="96"/>
+      <c r="IK23" s="96"/>
+      <c r="IM23" s="96"/>
+      <c r="IN23" s="96"/>
+      <c r="IO23" s="96"/>
+      <c r="IP23" s="96"/>
+      <c r="IQ23" s="96"/>
+      <c r="IS23" s="96"/>
+      <c r="IT23" s="97"/>
+      <c r="IU23" s="97"/>
     </row>
   </sheetData>
   <mergeCells count="172">
-    <mergeCell ref="IM23:IQ23"/>
-    <mergeCell ref="IS23:IU23"/>
-    <mergeCell ref="HC23:HG23"/>
-    <mergeCell ref="HI23:HM23"/>
-    <mergeCell ref="HO23:HS23"/>
-    <mergeCell ref="HU23:HY23"/>
-    <mergeCell ref="IA23:IE23"/>
-    <mergeCell ref="IG23:IK23"/>
-    <mergeCell ref="FS23:FW23"/>
-    <mergeCell ref="FY23:GC23"/>
-    <mergeCell ref="GE23:GI23"/>
-    <mergeCell ref="GK23:GO23"/>
-    <mergeCell ref="GQ23:GU23"/>
-    <mergeCell ref="GW23:HA23"/>
-    <mergeCell ref="EI23:EM23"/>
-    <mergeCell ref="EO23:ES23"/>
-    <mergeCell ref="EU23:EY23"/>
-    <mergeCell ref="FA23:FE23"/>
-    <mergeCell ref="FG23:FK23"/>
-    <mergeCell ref="FM23:FQ23"/>
-    <mergeCell ref="CY23:DC23"/>
-    <mergeCell ref="DE23:DI23"/>
-    <mergeCell ref="DK23:DO23"/>
-    <mergeCell ref="DQ23:DU23"/>
-    <mergeCell ref="DW23:EA23"/>
-    <mergeCell ref="EC23:EG23"/>
-    <mergeCell ref="BO23:BS23"/>
-    <mergeCell ref="BU23:BY23"/>
-    <mergeCell ref="CA23:CE23"/>
-    <mergeCell ref="CG23:CK23"/>
-    <mergeCell ref="CM23:CQ23"/>
-    <mergeCell ref="CS23:CW23"/>
-    <mergeCell ref="AE23:AI23"/>
-    <mergeCell ref="AK23:AO23"/>
-    <mergeCell ref="AQ23:AU23"/>
-    <mergeCell ref="AW23:BA23"/>
-    <mergeCell ref="BC23:BG23"/>
-    <mergeCell ref="BI23:BM23"/>
-    <mergeCell ref="HO21:HS21"/>
-    <mergeCell ref="HU21:HY21"/>
-    <mergeCell ref="IA21:IE21"/>
-    <mergeCell ref="IG21:IK21"/>
-    <mergeCell ref="IM21:IQ21"/>
-    <mergeCell ref="IS21:IU21"/>
-    <mergeCell ref="GE21:GI21"/>
-    <mergeCell ref="GK21:GO21"/>
-    <mergeCell ref="GQ21:GU21"/>
-    <mergeCell ref="GW21:HA21"/>
-    <mergeCell ref="HC21:HG21"/>
-    <mergeCell ref="HI21:HM21"/>
-    <mergeCell ref="EU21:EY21"/>
-    <mergeCell ref="FA21:FE21"/>
-    <mergeCell ref="FG21:FK21"/>
-    <mergeCell ref="FM21:FQ21"/>
-    <mergeCell ref="FS21:FW21"/>
-    <mergeCell ref="FY21:GC21"/>
-    <mergeCell ref="DK21:DO21"/>
-    <mergeCell ref="DQ21:DU21"/>
-    <mergeCell ref="DW21:EA21"/>
-    <mergeCell ref="EC21:EG21"/>
-    <mergeCell ref="EI21:EM21"/>
-    <mergeCell ref="EO21:ES21"/>
-    <mergeCell ref="CG21:CK21"/>
-    <mergeCell ref="CM21:CQ21"/>
-    <mergeCell ref="CS21:CW21"/>
-    <mergeCell ref="CY21:DC21"/>
-    <mergeCell ref="DE21:DI21"/>
-    <mergeCell ref="AQ21:AU21"/>
-    <mergeCell ref="AW21:BA21"/>
-    <mergeCell ref="BC21:BG21"/>
-    <mergeCell ref="BI21:BM21"/>
-    <mergeCell ref="BO21:BS21"/>
-    <mergeCell ref="BU21:BY21"/>
+    <mergeCell ref="AE1:AI1"/>
+    <mergeCell ref="AK1:AO1"/>
+    <mergeCell ref="AQ1:AU1"/>
+    <mergeCell ref="AW1:BA1"/>
+    <mergeCell ref="BC1:BG1"/>
+    <mergeCell ref="BI1:BM1"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="M1:Q1"/>
+    <mergeCell ref="S1:W1"/>
+    <mergeCell ref="Y1:AC1"/>
+    <mergeCell ref="G23:K23"/>
+    <mergeCell ref="M23:Q23"/>
+    <mergeCell ref="S23:W23"/>
+    <mergeCell ref="Y23:AC23"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="BC19:BG19"/>
+    <mergeCell ref="BI19:BM19"/>
+    <mergeCell ref="CY1:DC1"/>
+    <mergeCell ref="DE1:DI1"/>
+    <mergeCell ref="DK1:DO1"/>
+    <mergeCell ref="DQ1:DU1"/>
+    <mergeCell ref="DW1:EA1"/>
+    <mergeCell ref="EC1:EG1"/>
+    <mergeCell ref="BO1:BS1"/>
+    <mergeCell ref="BU1:BY1"/>
+    <mergeCell ref="CA1:CE1"/>
+    <mergeCell ref="CG1:CK1"/>
+    <mergeCell ref="CM1:CQ1"/>
+    <mergeCell ref="CS1:CW1"/>
+    <mergeCell ref="GE1:GI1"/>
+    <mergeCell ref="GK1:GO1"/>
+    <mergeCell ref="GQ1:GU1"/>
+    <mergeCell ref="GW1:HA1"/>
+    <mergeCell ref="EI1:EM1"/>
+    <mergeCell ref="EO1:ES1"/>
+    <mergeCell ref="EU1:EY1"/>
+    <mergeCell ref="FA1:FE1"/>
+    <mergeCell ref="FG1:FK1"/>
+    <mergeCell ref="FM1:FQ1"/>
+    <mergeCell ref="BO19:BS19"/>
+    <mergeCell ref="BU19:BY19"/>
+    <mergeCell ref="CA19:CE19"/>
+    <mergeCell ref="CG19:CK19"/>
+    <mergeCell ref="IM1:IQ1"/>
+    <mergeCell ref="IS1:IU1"/>
+    <mergeCell ref="G19:K19"/>
+    <mergeCell ref="M19:Q19"/>
+    <mergeCell ref="S19:W19"/>
+    <mergeCell ref="Y19:AC19"/>
+    <mergeCell ref="AE19:AI19"/>
+    <mergeCell ref="AK19:AO19"/>
+    <mergeCell ref="AQ19:AU19"/>
+    <mergeCell ref="AW19:BA19"/>
+    <mergeCell ref="HC1:HG1"/>
+    <mergeCell ref="HI1:HM1"/>
+    <mergeCell ref="HO1:HS1"/>
+    <mergeCell ref="HU1:HY1"/>
+    <mergeCell ref="IA1:IE1"/>
+    <mergeCell ref="IG1:IK1"/>
+    <mergeCell ref="FS1:FW1"/>
+    <mergeCell ref="FY1:GC1"/>
+    <mergeCell ref="EI19:EM19"/>
+    <mergeCell ref="EO19:ES19"/>
+    <mergeCell ref="EU19:EY19"/>
+    <mergeCell ref="FA19:FE19"/>
+    <mergeCell ref="CM19:CQ19"/>
+    <mergeCell ref="CS19:CW19"/>
+    <mergeCell ref="CY19:DC19"/>
+    <mergeCell ref="DE19:DI19"/>
+    <mergeCell ref="DK19:DO19"/>
+    <mergeCell ref="DQ19:DU19"/>
+    <mergeCell ref="IA19:IE19"/>
     <mergeCell ref="IG19:IK19"/>
     <mergeCell ref="IM19:IQ19"/>
     <mergeCell ref="IS19:IU19"/>
@@ -3976,81 +3980,79 @@
     <mergeCell ref="DW19:EA19"/>
     <mergeCell ref="EC19:EG19"/>
     <mergeCell ref="CA21:CE21"/>
-    <mergeCell ref="EU19:EY19"/>
-    <mergeCell ref="FA19:FE19"/>
-    <mergeCell ref="CM19:CQ19"/>
-    <mergeCell ref="CS19:CW19"/>
-    <mergeCell ref="CY19:DC19"/>
-    <mergeCell ref="DE19:DI19"/>
-    <mergeCell ref="DK19:DO19"/>
-    <mergeCell ref="DQ19:DU19"/>
-    <mergeCell ref="IA19:IE19"/>
-    <mergeCell ref="BO19:BS19"/>
-    <mergeCell ref="BU19:BY19"/>
-    <mergeCell ref="CA19:CE19"/>
-    <mergeCell ref="CG19:CK19"/>
-    <mergeCell ref="IM1:IQ1"/>
-    <mergeCell ref="IS1:IU1"/>
-    <mergeCell ref="G19:K19"/>
-    <mergeCell ref="M19:Q19"/>
-    <mergeCell ref="S19:W19"/>
-    <mergeCell ref="Y19:AC19"/>
-    <mergeCell ref="AE19:AI19"/>
-    <mergeCell ref="AK19:AO19"/>
-    <mergeCell ref="AQ19:AU19"/>
-    <mergeCell ref="AW19:BA19"/>
-    <mergeCell ref="HC1:HG1"/>
-    <mergeCell ref="HI1:HM1"/>
-    <mergeCell ref="HO1:HS1"/>
-    <mergeCell ref="HU1:HY1"/>
-    <mergeCell ref="IA1:IE1"/>
-    <mergeCell ref="IG1:IK1"/>
-    <mergeCell ref="FS1:FW1"/>
-    <mergeCell ref="FY1:GC1"/>
-    <mergeCell ref="EI19:EM19"/>
-    <mergeCell ref="EO19:ES19"/>
-    <mergeCell ref="GE1:GI1"/>
-    <mergeCell ref="GK1:GO1"/>
-    <mergeCell ref="GQ1:GU1"/>
-    <mergeCell ref="GW1:HA1"/>
-    <mergeCell ref="EI1:EM1"/>
-    <mergeCell ref="EO1:ES1"/>
-    <mergeCell ref="EU1:EY1"/>
-    <mergeCell ref="FA1:FE1"/>
-    <mergeCell ref="FG1:FK1"/>
-    <mergeCell ref="FM1:FQ1"/>
-    <mergeCell ref="CY1:DC1"/>
-    <mergeCell ref="DE1:DI1"/>
-    <mergeCell ref="DK1:DO1"/>
-    <mergeCell ref="DQ1:DU1"/>
-    <mergeCell ref="DW1:EA1"/>
-    <mergeCell ref="EC1:EG1"/>
-    <mergeCell ref="BO1:BS1"/>
-    <mergeCell ref="BU1:BY1"/>
-    <mergeCell ref="CA1:CE1"/>
-    <mergeCell ref="CG1:CK1"/>
-    <mergeCell ref="CM1:CQ1"/>
-    <mergeCell ref="CS1:CW1"/>
-    <mergeCell ref="AE1:AI1"/>
-    <mergeCell ref="AK1:AO1"/>
-    <mergeCell ref="AQ1:AU1"/>
-    <mergeCell ref="AW1:BA1"/>
-    <mergeCell ref="BC1:BG1"/>
-    <mergeCell ref="BI1:BM1"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="G1:K1"/>
-    <mergeCell ref="M1:Q1"/>
-    <mergeCell ref="S1:W1"/>
-    <mergeCell ref="Y1:AC1"/>
-    <mergeCell ref="G23:K23"/>
-    <mergeCell ref="M23:Q23"/>
-    <mergeCell ref="S23:W23"/>
-    <mergeCell ref="Y23:AC23"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="BC19:BG19"/>
-    <mergeCell ref="BI19:BM19"/>
+    <mergeCell ref="CG21:CK21"/>
+    <mergeCell ref="CM21:CQ21"/>
+    <mergeCell ref="CS21:CW21"/>
+    <mergeCell ref="CY21:DC21"/>
+    <mergeCell ref="DE21:DI21"/>
+    <mergeCell ref="AQ21:AU21"/>
+    <mergeCell ref="AW21:BA21"/>
+    <mergeCell ref="BC21:BG21"/>
+    <mergeCell ref="BI21:BM21"/>
+    <mergeCell ref="BO21:BS21"/>
+    <mergeCell ref="BU21:BY21"/>
+    <mergeCell ref="EU21:EY21"/>
+    <mergeCell ref="FA21:FE21"/>
+    <mergeCell ref="FG21:FK21"/>
+    <mergeCell ref="FM21:FQ21"/>
+    <mergeCell ref="FS21:FW21"/>
+    <mergeCell ref="FY21:GC21"/>
+    <mergeCell ref="DK21:DO21"/>
+    <mergeCell ref="DQ21:DU21"/>
+    <mergeCell ref="DW21:EA21"/>
+    <mergeCell ref="EC21:EG21"/>
+    <mergeCell ref="EI21:EM21"/>
+    <mergeCell ref="EO21:ES21"/>
+    <mergeCell ref="HO21:HS21"/>
+    <mergeCell ref="HU21:HY21"/>
+    <mergeCell ref="IA21:IE21"/>
+    <mergeCell ref="IG21:IK21"/>
+    <mergeCell ref="IM21:IQ21"/>
+    <mergeCell ref="IS21:IU21"/>
+    <mergeCell ref="GE21:GI21"/>
+    <mergeCell ref="GK21:GO21"/>
+    <mergeCell ref="GQ21:GU21"/>
+    <mergeCell ref="GW21:HA21"/>
+    <mergeCell ref="HC21:HG21"/>
+    <mergeCell ref="HI21:HM21"/>
+    <mergeCell ref="BO23:BS23"/>
+    <mergeCell ref="BU23:BY23"/>
+    <mergeCell ref="CA23:CE23"/>
+    <mergeCell ref="CG23:CK23"/>
+    <mergeCell ref="CM23:CQ23"/>
+    <mergeCell ref="CS23:CW23"/>
+    <mergeCell ref="AE23:AI23"/>
+    <mergeCell ref="AK23:AO23"/>
+    <mergeCell ref="AQ23:AU23"/>
+    <mergeCell ref="AW23:BA23"/>
+    <mergeCell ref="BC23:BG23"/>
+    <mergeCell ref="BI23:BM23"/>
+    <mergeCell ref="EI23:EM23"/>
+    <mergeCell ref="EO23:ES23"/>
+    <mergeCell ref="EU23:EY23"/>
+    <mergeCell ref="FA23:FE23"/>
+    <mergeCell ref="FG23:FK23"/>
+    <mergeCell ref="FM23:FQ23"/>
+    <mergeCell ref="CY23:DC23"/>
+    <mergeCell ref="DE23:DI23"/>
+    <mergeCell ref="DK23:DO23"/>
+    <mergeCell ref="DQ23:DU23"/>
+    <mergeCell ref="DW23:EA23"/>
+    <mergeCell ref="EC23:EG23"/>
+    <mergeCell ref="IM23:IQ23"/>
+    <mergeCell ref="IS23:IU23"/>
+    <mergeCell ref="HC23:HG23"/>
+    <mergeCell ref="HI23:HM23"/>
+    <mergeCell ref="HO23:HS23"/>
+    <mergeCell ref="HU23:HY23"/>
+    <mergeCell ref="IA23:IE23"/>
+    <mergeCell ref="IG23:IK23"/>
+    <mergeCell ref="FS23:FW23"/>
+    <mergeCell ref="FY23:GC23"/>
+    <mergeCell ref="GE23:GI23"/>
+    <mergeCell ref="GK23:GO23"/>
+    <mergeCell ref="GQ23:GU23"/>
+    <mergeCell ref="GW23:HA23"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C6" location="Issuance!A1" display="US Corporate Bonds: Issuance" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -4068,11 +4070,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:X54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="8" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="A47" sqref="A47"/>
+      <selection pane="bottomRight" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
@@ -7104,7 +7106,7 @@
       <pane xSplit="1" ySplit="8" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="A47" sqref="A47"/>
+      <selection pane="bottomRight" activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>

</xml_diff>